<commit_message>
changed refinement levels in current test runsx
</commit_message>
<xml_diff>
--- a/RefinementLevels.xlsx
+++ b/RefinementLevels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cathe\PycharmProjects\BarrierIslandBreach\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherinej/projects/BarrierIslandBreach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDBAC342-A8E1-4426-A24E-7630C9CA0587}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9309BF-0AA0-2D49-95F4-72D033455193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1833" yWindow="1833" windowWidth="19200" windowHeight="10074" xr2:uid="{555F1360-F659-4008-A3EA-3F5DA8A630E5}"/>
+    <workbookView xWindow="1840" yWindow="1840" windowWidth="22720" windowHeight="12920" xr2:uid="{555F1360-F659-4008-A3EA-3F5DA8A630E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
   <si>
     <t>Total Lat</t>
   </si>
@@ -94,12 +88,21 @@
   </si>
   <si>
     <t>East</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40.819273°</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40.817693°</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000000000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -137,9 +140,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -454,23 +458,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393A34C5-94AD-4C93-B649-F37F7B1F6742}">
-  <dimension ref="A1:O25"/>
+  <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="5" max="5" width="13.1640625" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="0" hidden="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>17</v>
       </c>
@@ -484,39 +489,39 @@
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A3">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="B3">
-        <v>32</v>
+        <v>45</v>
       </c>
       <c r="C3">
-        <v>-99</v>
+        <v>-85</v>
       </c>
       <c r="D3">
-        <v>-70</v>
-      </c>
-    </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.5">
+        <v>-55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>0</v>
       </c>
       <c r="B5">
         <f>B3-A3</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>1</v>
       </c>
       <c r="B6">
         <f>D3-C3</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>13</v>
       </c>
@@ -554,17 +559,17 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>2</v>
       </c>
       <c r="B8">
         <f>4*B6</f>
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="C8">
         <f>B8</f>
-        <v>116</v>
+        <v>120</v>
       </c>
       <c r="D8">
         <f>$B$6/B8</f>
@@ -586,12 +591,12 @@
         <v>2</v>
       </c>
       <c r="J8">
-        <f>4*12</f>
-        <v>48</v>
+        <f>B5*4</f>
+        <v>128</v>
       </c>
       <c r="K8">
         <f>J8</f>
-        <v>48</v>
+        <v>128</v>
       </c>
       <c r="L8">
         <f>$B$5/J8</f>
@@ -610,115 +615,115 @@
         <v>27000</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.5">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C9">
         <f t="shared" ref="C9:C14" si="0">C8*B9</f>
-        <v>464</v>
+        <v>240</v>
       </c>
       <c r="D9">
         <f t="shared" ref="D9:D14" si="1">D8/B9</f>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
       <c r="E9">
         <f t="shared" ref="E9:F14" si="2">D9*60</f>
-        <v>3.75</v>
+        <v>7.5</v>
       </c>
       <c r="F9">
         <f t="shared" si="2"/>
-        <v>225</v>
+        <v>450</v>
       </c>
       <c r="G9">
         <f t="shared" ref="G9:G14" si="3">F9*30</f>
-        <v>6750</v>
+        <v>13500</v>
       </c>
       <c r="I9" t="s">
         <v>7</v>
       </c>
       <c r="J9">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K9">
         <f t="shared" ref="K9:K14" si="4">K8*J9</f>
-        <v>192</v>
+        <v>256</v>
       </c>
       <c r="L9">
         <f t="shared" ref="L9:L14" si="5">L8/J9</f>
-        <v>6.25E-2</v>
+        <v>0.125</v>
       </c>
       <c r="M9">
         <f t="shared" ref="M9:N9" si="6">L9*60</f>
-        <v>3.75</v>
+        <v>7.5</v>
       </c>
       <c r="N9">
         <f t="shared" si="6"/>
-        <v>225</v>
+        <v>450</v>
       </c>
       <c r="O9">
         <f t="shared" ref="O9:O14" si="7">N9*30</f>
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.5">
+        <v>13500</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="C10">
         <f t="shared" si="0"/>
-        <v>1856</v>
+        <v>480</v>
       </c>
       <c r="D10">
         <f t="shared" si="1"/>
-        <v>1.5625E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="E10">
         <f t="shared" si="2"/>
-        <v>0.9375</v>
+        <v>3.75</v>
       </c>
       <c r="F10">
         <f t="shared" si="2"/>
-        <v>56.25</v>
+        <v>225</v>
       </c>
       <c r="G10">
         <f t="shared" si="3"/>
-        <v>1687.5</v>
+        <v>6750</v>
       </c>
       <c r="I10" t="s">
         <v>8</v>
       </c>
       <c r="J10">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K10">
         <f t="shared" si="4"/>
-        <v>768</v>
+        <v>512</v>
       </c>
       <c r="L10">
         <f t="shared" si="5"/>
-        <v>1.5625E-2</v>
+        <v>6.25E-2</v>
       </c>
       <c r="M10">
         <f t="shared" ref="M10:N10" si="8">L10*60</f>
-        <v>0.9375</v>
+        <v>3.75</v>
       </c>
       <c r="N10">
         <f t="shared" si="8"/>
-        <v>56.25</v>
+        <v>225</v>
       </c>
       <c r="O10">
         <f t="shared" si="7"/>
-        <v>1687.5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.5">
+        <v>6750</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -727,23 +732,23 @@
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>9280</v>
+        <v>2400</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>3.1250000000000002E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>0.1875</v>
+        <v>0.75</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>11.25</v>
+        <v>45</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>337.5</v>
+        <v>1350</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
@@ -753,206 +758,206 @@
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>3840</v>
+        <v>2560</v>
       </c>
       <c r="L11">
         <f t="shared" si="5"/>
-        <v>3.1250000000000002E-3</v>
+        <v>1.2500000000000001E-2</v>
       </c>
       <c r="M11">
         <f t="shared" ref="M11:N11" si="9">L11*60</f>
-        <v>0.1875</v>
+        <v>0.75</v>
       </c>
       <c r="N11">
         <f t="shared" si="9"/>
-        <v>11.25</v>
+        <v>45</v>
       </c>
       <c r="O11">
         <f t="shared" si="7"/>
-        <v>337.5</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.5">
+        <v>1350</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>10</v>
       </c>
       <c r="B12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>111360</v>
+        <v>26400</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>2.6041666666666666E-4</v>
+        <v>1.1363636363636365E-3</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>1.5625E-2</v>
+        <v>6.8181818181818191E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>0.9375</v>
+        <v>4.0909090909090917</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>28.125</v>
+        <v>122.72727272727275</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
       </c>
       <c r="J12">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>46080</v>
+        <v>28160</v>
       </c>
       <c r="L12">
         <f t="shared" si="5"/>
-        <v>2.6041666666666666E-4</v>
+        <v>1.1363636363636365E-3</v>
       </c>
       <c r="M12">
         <f t="shared" ref="M12:N12" si="10">L12*60</f>
-        <v>1.5625E-2</v>
+        <v>6.8181818181818191E-2</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
-        <v>0.9375</v>
+        <v>4.0909090909090917</v>
       </c>
       <c r="O12">
         <f t="shared" si="7"/>
-        <v>28.125</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.5">
+        <v>122.72727272727275</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>11</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>1113600</v>
+        <v>105600</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>2.6041666666666665E-5</v>
+        <v>2.8409090909090913E-4</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>1.5624999999999999E-3</v>
+        <v>1.7045454545454548E-2</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>9.3749999999999986E-2</v>
+        <v>1.0227272727272729</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>2.8124999999999996</v>
+        <v>30.681818181818187</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="J13">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>460800</v>
+        <v>112640</v>
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>2.6041666666666665E-5</v>
+        <v>2.8409090909090913E-4</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13:N13" si="11">L13*60</f>
-        <v>1.5624999999999999E-3</v>
+        <v>1.7045454545454548E-2</v>
       </c>
       <c r="N13">
         <f t="shared" si="11"/>
-        <v>9.3749999999999986E-2</v>
+        <v>1.0227272727272729</v>
       </c>
       <c r="O13">
         <f t="shared" si="7"/>
-        <v>2.8124999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.5">
+        <v>30.681818181818187</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>12</v>
       </c>
       <c r="B14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>2227200</v>
+        <v>633600</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>1.3020833333333332E-5</v>
+        <v>4.7348484848484855E-5</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>7.8124999999999993E-4</v>
+        <v>2.8409090909090914E-3</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>4.6874999999999993E-2</v>
+        <v>0.1704545454545455</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>1.4062499999999998</v>
+        <v>5.1136363636363651</v>
       </c>
       <c r="I14" t="s">
         <v>12</v>
       </c>
       <c r="J14">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>921600</v>
+        <v>675840</v>
       </c>
       <c r="L14">
         <f t="shared" si="5"/>
-        <v>1.3020833333333332E-5</v>
+        <v>4.7348484848484855E-5</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:N14" si="12">L14*60</f>
-        <v>7.8124999999999993E-4</v>
+        <v>2.8409090909090914E-3</v>
       </c>
       <c r="N14">
         <f t="shared" si="12"/>
-        <v>4.6874999999999993E-2</v>
+        <v>0.1704545454545455</v>
       </c>
       <c r="O14">
         <f t="shared" si="7"/>
-        <v>1.4062499999999998</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.5">
+        <v>5.1136363636363651</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>0</v>
       </c>
       <c r="B16">
         <f>B3-A3</f>
-        <v>12</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
       <c r="B17">
         <f>D3-C3</f>
-        <v>29</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.5">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -972,7 +977,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.5">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -985,22 +990,22 @@
       </c>
       <c r="D19">
         <f>$B$6/B19</f>
-        <v>1</v>
+        <v>1.0344827586206897</v>
       </c>
       <c r="E19">
         <f>D19*60</f>
-        <v>60</v>
+        <v>62.068965517241381</v>
       </c>
       <c r="F19">
         <f>E19*60</f>
-        <v>3600</v>
+        <v>3724.1379310344828</v>
       </c>
       <c r="G19">
         <f>F19*30</f>
-        <v>108000</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.5">
+        <v>111724.13793103448</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1013,22 +1018,22 @@
       </c>
       <c r="D20">
         <f t="shared" ref="D20:D25" si="14">D19/B20</f>
-        <v>0.25</v>
+        <v>0.25862068965517243</v>
       </c>
       <c r="E20">
         <f t="shared" ref="E20:E25" si="15">D20*60</f>
-        <v>15</v>
+        <v>15.517241379310345</v>
       </c>
       <c r="F20">
         <f t="shared" ref="F20:F25" si="16">E20*60</f>
-        <v>900</v>
+        <v>931.0344827586207</v>
       </c>
       <c r="G20">
         <f t="shared" ref="G20:G25" si="17">F20*30</f>
-        <v>27000</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.5">
+        <v>27931.03448275862</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1041,22 +1046,22 @@
       </c>
       <c r="D21">
         <f t="shared" si="14"/>
-        <v>6.25E-2</v>
+        <v>6.4655172413793108E-2</v>
       </c>
       <c r="E21">
         <f t="shared" si="15"/>
-        <v>3.75</v>
+        <v>3.8793103448275863</v>
       </c>
       <c r="F21">
         <f t="shared" si="16"/>
-        <v>225</v>
+        <v>232.75862068965517</v>
       </c>
       <c r="G21">
         <f t="shared" si="17"/>
-        <v>6750</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.5">
+        <v>6982.7586206896549</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1069,22 +1074,22 @@
       </c>
       <c r="D22">
         <f t="shared" si="14"/>
-        <v>1.2500000000000001E-2</v>
+        <v>1.2931034482758622E-2</v>
       </c>
       <c r="E22">
         <f t="shared" si="15"/>
-        <v>0.75</v>
+        <v>0.77586206896551735</v>
       </c>
       <c r="F22">
         <f t="shared" si="16"/>
-        <v>45</v>
+        <v>46.551724137931039</v>
       </c>
       <c r="G22">
         <f t="shared" si="17"/>
-        <v>1350</v>
-      </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.5">
+        <v>1396.5517241379312</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1097,22 +1102,22 @@
       </c>
       <c r="D23">
         <f t="shared" si="14"/>
-        <v>3.1250000000000002E-3</v>
+        <v>3.2327586206896556E-3</v>
       </c>
       <c r="E23">
         <f t="shared" si="15"/>
-        <v>0.1875</v>
+        <v>0.19396551724137934</v>
       </c>
       <c r="F23">
         <f t="shared" si="16"/>
-        <v>11.25</v>
+        <v>11.63793103448276</v>
       </c>
       <c r="G23">
         <f t="shared" si="17"/>
-        <v>337.5</v>
-      </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.5">
+        <v>349.13793103448279</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1125,22 +1130,22 @@
       </c>
       <c r="D24">
         <f t="shared" si="14"/>
-        <v>3.1250000000000001E-4</v>
+        <v>3.2327586206896557E-4</v>
       </c>
       <c r="E24">
         <f t="shared" si="15"/>
-        <v>1.8749999999999999E-2</v>
+        <v>1.9396551724137935E-2</v>
       </c>
       <c r="F24">
         <f t="shared" si="16"/>
-        <v>1.125</v>
+        <v>1.163793103448276</v>
       </c>
       <c r="G24">
         <f t="shared" si="17"/>
-        <v>33.75</v>
-      </c>
-    </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.5">
+        <v>34.913793103448278</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1153,19 +1158,47 @@
       </c>
       <c r="D25">
         <f t="shared" si="14"/>
-        <v>1.5625E-4</v>
+        <v>1.6163793103448278E-4</v>
       </c>
       <c r="E25">
         <f t="shared" si="15"/>
-        <v>9.3749999999999997E-3</v>
+        <v>9.6982758620689676E-3</v>
       </c>
       <c r="F25">
         <f t="shared" si="16"/>
-        <v>0.5625</v>
+        <v>0.58189655172413801</v>
       </c>
       <c r="G25">
         <f t="shared" si="17"/>
-        <v>16.875</v>
+        <v>17.456896551724139</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E28">
+        <f>300/3600/60</f>
+        <v>1.3888888888888887E-3</v>
+      </c>
+      <c r="G28" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="D29">
+        <f>-72.56</f>
+        <v>-72.56</v>
+      </c>
+      <c r="E29" s="2">
+        <f>D29+E28</f>
+        <v>-72.558611111111119</v>
+      </c>
+      <c r="G29" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="E30" s="2">
+        <f>D29-E28</f>
+        <v>-72.561388888888885</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated .gitignore to ignore .DS_Store and .ipynb checkpoints
</commit_message>
<xml_diff>
--- a/RefinementLevels.xlsx
+++ b/RefinementLevels.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11213"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/catherinej/projects/BarrierIslandBreach/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB9309BF-0AA0-2D49-95F4-72D033455193}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8355A27E-529B-494A-9AD2-979C21D26D4F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1840" yWindow="1840" windowWidth="22720" windowHeight="12920" xr2:uid="{555F1360-F659-4008-A3EA-3F5DA8A630E5}"/>
+    <workbookView xWindow="9520" yWindow="3220" windowWidth="22720" windowHeight="12920" xr2:uid="{555F1360-F659-4008-A3EA-3F5DA8A630E5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="25">
   <si>
     <t>Total Lat</t>
   </si>
@@ -94,6 +94,12 @@
   </si>
   <si>
     <t xml:space="preserve"> 40.817693°</t>
+  </si>
+  <si>
+    <t>forcing the depth, copy the boundaries into the domain then set the depth</t>
+  </si>
+  <si>
+    <t>set the height and depth based on the tide</t>
   </si>
 </sst>
 </file>
@@ -460,8 +466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{393A34C5-94AD-4C93-B649-F37F7B1F6742}">
   <dimension ref="A1:O30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -587,6 +593,10 @@
         <f>F8*30</f>
         <v>27000</v>
       </c>
+      <c r="H8">
+        <f>G8/15</f>
+        <v>1800</v>
+      </c>
       <c r="I8" t="s">
         <v>2</v>
       </c>
@@ -728,53 +738,53 @@
         <v>9</v>
       </c>
       <c r="B11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C11">
         <f t="shared" si="0"/>
-        <v>2400</v>
+        <v>2880</v>
       </c>
       <c r="D11">
         <f t="shared" si="1"/>
-        <v>1.2500000000000001E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="E11">
         <f t="shared" si="2"/>
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="F11">
         <f t="shared" si="2"/>
-        <v>45</v>
+        <v>37.5</v>
       </c>
       <c r="G11">
         <f t="shared" si="3"/>
-        <v>1350</v>
+        <v>1125</v>
       </c>
       <c r="I11" t="s">
         <v>9</v>
       </c>
       <c r="J11">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K11">
         <f t="shared" si="4"/>
-        <v>2560</v>
+        <v>3072</v>
       </c>
       <c r="L11">
         <f t="shared" si="5"/>
-        <v>1.2500000000000001E-2</v>
+        <v>1.0416666666666666E-2</v>
       </c>
       <c r="M11">
         <f t="shared" ref="M11:N11" si="9">L11*60</f>
-        <v>0.75</v>
+        <v>0.625</v>
       </c>
       <c r="N11">
         <f t="shared" si="9"/>
-        <v>45</v>
+        <v>37.5</v>
       </c>
       <c r="O11">
         <f t="shared" si="7"/>
-        <v>1350</v>
+        <v>1125</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.2">
@@ -782,27 +792,27 @@
         <v>10</v>
       </c>
       <c r="B12">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="C12">
         <f t="shared" si="0"/>
-        <v>26400</v>
+        <v>20160</v>
       </c>
       <c r="D12">
         <f t="shared" si="1"/>
-        <v>1.1363636363636365E-3</v>
+        <v>1.488095238095238E-3</v>
       </c>
       <c r="E12">
         <f t="shared" si="2"/>
-        <v>6.8181818181818191E-2</v>
+        <v>8.9285714285714274E-2</v>
       </c>
       <c r="F12">
         <f t="shared" si="2"/>
-        <v>4.0909090909090917</v>
+        <v>5.3571428571428568</v>
       </c>
       <c r="G12">
         <f t="shared" si="3"/>
-        <v>122.72727272727275</v>
+        <v>160.71428571428569</v>
       </c>
       <c r="I12" t="s">
         <v>10</v>
@@ -812,23 +822,23 @@
       </c>
       <c r="K12">
         <f t="shared" si="4"/>
-        <v>28160</v>
+        <v>33792</v>
       </c>
       <c r="L12">
         <f t="shared" si="5"/>
-        <v>1.1363636363636365E-3</v>
+        <v>9.4696969696969689E-4</v>
       </c>
       <c r="M12">
         <f t="shared" ref="M12:N12" si="10">L12*60</f>
-        <v>6.8181818181818191E-2</v>
+        <v>5.6818181818181816E-2</v>
       </c>
       <c r="N12">
         <f t="shared" si="10"/>
-        <v>4.0909090909090917</v>
+        <v>3.4090909090909092</v>
       </c>
       <c r="O12">
         <f t="shared" si="7"/>
-        <v>122.72727272727275</v>
+        <v>102.27272727272728</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.2">
@@ -836,53 +846,53 @@
         <v>11</v>
       </c>
       <c r="B13">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="C13">
         <f t="shared" si="0"/>
-        <v>105600</v>
+        <v>221760</v>
       </c>
       <c r="D13">
         <f t="shared" si="1"/>
-        <v>2.8409090909090913E-4</v>
+        <v>1.3528138528138528E-4</v>
       </c>
       <c r="E13">
         <f t="shared" si="2"/>
-        <v>1.7045454545454548E-2</v>
+        <v>8.1168831168831161E-3</v>
       </c>
       <c r="F13">
         <f t="shared" si="2"/>
-        <v>1.0227272727272729</v>
+        <v>0.48701298701298695</v>
       </c>
       <c r="G13">
         <f t="shared" si="3"/>
-        <v>30.681818181818187</v>
+        <v>14.610389610389609</v>
       </c>
       <c r="I13" t="s">
         <v>11</v>
       </c>
       <c r="J13">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="K13">
         <f t="shared" si="4"/>
-        <v>112640</v>
+        <v>67584</v>
       </c>
       <c r="L13">
         <f t="shared" si="5"/>
-        <v>2.8409090909090913E-4</v>
+        <v>4.7348484848484844E-4</v>
       </c>
       <c r="M13">
         <f t="shared" ref="M13:N13" si="11">L13*60</f>
-        <v>1.7045454545454548E-2</v>
+        <v>2.8409090909090908E-2</v>
       </c>
       <c r="N13">
         <f t="shared" si="11"/>
-        <v>1.0227272727272729</v>
+        <v>1.7045454545454546</v>
       </c>
       <c r="O13">
         <f t="shared" si="7"/>
-        <v>30.681818181818187</v>
+        <v>51.13636363636364</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.2">
@@ -890,53 +900,53 @@
         <v>12</v>
       </c>
       <c r="B14">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
-        <v>633600</v>
+        <v>443520</v>
       </c>
       <c r="D14">
         <f t="shared" si="1"/>
-        <v>4.7348484848484855E-5</v>
+        <v>6.7640692640692641E-5</v>
       </c>
       <c r="E14">
         <f t="shared" si="2"/>
-        <v>2.8409090909090914E-3</v>
+        <v>4.0584415584415581E-3</v>
       </c>
       <c r="F14">
         <f t="shared" si="2"/>
-        <v>0.1704545454545455</v>
+        <v>0.24350649350649348</v>
       </c>
       <c r="G14">
         <f t="shared" si="3"/>
-        <v>5.1136363636363651</v>
+        <v>7.3051948051948044</v>
       </c>
       <c r="I14" t="s">
         <v>12</v>
       </c>
       <c r="J14">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K14">
         <f t="shared" si="4"/>
-        <v>675840</v>
+        <v>337920</v>
       </c>
       <c r="L14">
         <f t="shared" si="5"/>
-        <v>4.7348484848484855E-5</v>
+        <v>9.4696969696969683E-5</v>
       </c>
       <c r="M14">
         <f t="shared" ref="M14:N14" si="12">L14*60</f>
-        <v>2.8409090909090914E-3</v>
+        <v>5.6818181818181811E-3</v>
       </c>
       <c r="N14">
         <f t="shared" si="12"/>
-        <v>0.1704545454545455</v>
+        <v>0.34090909090909088</v>
       </c>
       <c r="O14">
         <f t="shared" si="7"/>
-        <v>5.1136363636363651</v>
+        <v>10.227272727272727</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.2">
@@ -948,7 +958,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>1</v>
       </c>
@@ -957,7 +967,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>13</v>
       </c>
@@ -977,7 +987,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>2</v>
       </c>
@@ -1005,7 +1015,7 @@
         <v>111724.13793103448</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>7</v>
       </c>
@@ -1033,7 +1043,7 @@
         <v>27931.03448275862</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>8</v>
       </c>
@@ -1060,8 +1070,11 @@
         <f t="shared" si="17"/>
         <v>6982.7586206896549</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L21" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>9</v>
       </c>
@@ -1088,8 +1101,11 @@
         <f t="shared" si="17"/>
         <v>1396.5517241379312</v>
       </c>
-    </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="L22" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -1117,7 +1133,7 @@
         <v>349.13793103448279</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>11</v>
       </c>
@@ -1145,7 +1161,7 @@
         <v>34.913793103448278</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>12</v>
       </c>
@@ -1173,7 +1189,7 @@
         <v>17.456896551724139</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E28">
         <f>300/3600/60</f>
         <v>1.3888888888888887E-3</v>
@@ -1182,7 +1198,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="D29">
         <f>-72.56</f>
         <v>-72.56</v>
@@ -1195,7 +1211,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E30" s="2">
         <f>D29-E28</f>
         <v>-72.561388888888885</v>

</xml_diff>